<commit_message>
test : cannot moving pawn across existing pawn
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
-    <t>atk</t>
-  </si>
-  <si>
     <t>3:0</t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>5:9</t>
+  </si>
+  <si>
+    <t>1:0</t>
   </si>
 </sst>
 </file>
@@ -900,7 +900,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,19 +952,19 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="6" t="s">
         <v>4</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>5</v>
       </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
@@ -980,7 +980,7 @@
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
       <c r="G3" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -1009,21 +1009,21 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1031,25 +1031,25 @@
         <v>4</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1057,33 +1057,33 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1091,25 +1091,25 @@
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1117,21 +1117,21 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
       <c r="G9" s="16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -1176,19 +1176,19 @@
       <c r="C12" s="31"/>
       <c r="D12" s="31"/>
       <c r="E12" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="G12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="H12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="34" t="s">
+      <c r="I12" s="32" t="s">
         <v>34</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>35</v>
       </c>
       <c r="J12" s="31"/>
       <c r="K12" s="31"/>

</xml_diff>

<commit_message>
debugging, solving @£%!§ copy code ><
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>3:0</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>1:0</t>
+  </si>
+  <si>
+    <t>4:1</t>
+  </si>
+  <si>
+    <t>targer</t>
+  </si>
+  <si>
+    <t>defensor</t>
   </si>
 </sst>
 </file>
@@ -897,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,7 +987,9 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
+      <c r="F3" s="16" t="s">
+        <v>37</v>
+      </c>
       <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1208,6 +1219,14 @@
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
     </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
optimizing CheckCapture by using a for loop
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
   <si>
     <t>3:0</t>
   </si>
@@ -137,13 +138,16 @@
     <t>1:0</t>
   </si>
   <si>
-    <t>4:1</t>
-  </si>
-  <si>
     <t>targer</t>
   </si>
   <si>
     <t>defensor</t>
+  </si>
+  <si>
+    <t>9:5 =&gt; 9:6</t>
+  </si>
+  <si>
+    <t>attacker</t>
   </si>
 </sst>
 </file>
@@ -516,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,6 +628,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -906,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,9 +995,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="16" t="s">
-        <v>37</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1004,7 +1010,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
+      <c r="C4" s="38"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -1023,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="38"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="16" t="s">
@@ -1083,21 +1089,14 @@
       <c r="G7" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>23</v>
-      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="25" t="s">
-        <v>29</v>
-      </c>
       <c r="L7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -1118,9 +1117,11 @@
       </c>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="28" t="s">
-        <v>27</v>
+      <c r="K8" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="23" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1221,10 +1222,342 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="37">
+        <v>0.42083333333333334</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
         <v>38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean effector -- clean simulate -- rename -delete analze
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -12,7 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="default (2)" sheetId="3" r:id="rId1"/>
+    <sheet name="default" sheetId="1" r:id="rId2"/>
+    <sheet name="calculs" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>3:0</t>
   </si>
@@ -135,12 +137,27 @@
   </si>
   <si>
     <t>1:0</t>
+  </si>
+  <si>
+    <t>mouvements simulés</t>
+  </si>
+  <si>
+    <t>mémoire :</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -507,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -617,6 +634,115 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,10 +1023,365 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P6" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" t="s">
+        <v>39</v>
+      </c>
+      <c r="P7" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="O8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:17" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:17" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I12" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L12" sqref="A1:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1212,4 +1693,435 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="33.85546875" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40">
+        <v>6</v>
+      </c>
+      <c r="F2" s="41">
+        <v>3</v>
+      </c>
+      <c r="G2" s="42">
+        <v>0</v>
+      </c>
+      <c r="H2" s="43">
+        <v>3</v>
+      </c>
+      <c r="I2" s="40">
+        <v>6</v>
+      </c>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="44"/>
+    </row>
+    <row r="3" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="47">
+        <v>11</v>
+      </c>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="48"/>
+    </row>
+    <row r="4" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="48"/>
+    </row>
+    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="49">
+        <v>6</v>
+      </c>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="50">
+        <v>9</v>
+      </c>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="52">
+        <v>3</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="50">
+        <v>6</v>
+      </c>
+      <c r="G6" s="53">
+        <v>0</v>
+      </c>
+      <c r="H6" s="50">
+        <v>6</v>
+      </c>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="42">
+        <v>0</v>
+      </c>
+      <c r="C7" s="55">
+        <v>11</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="50">
+        <v>9</v>
+      </c>
+      <c r="F7" s="56">
+        <v>0</v>
+      </c>
+      <c r="G7" s="57">
+        <v>0</v>
+      </c>
+      <c r="H7" s="58">
+        <v>0</v>
+      </c>
+      <c r="I7" s="50">
+        <v>9</v>
+      </c>
+      <c r="J7" s="46"/>
+      <c r="K7" s="59">
+        <v>11</v>
+      </c>
+      <c r="L7" s="42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="60">
+        <v>3</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="50">
+        <v>6</v>
+      </c>
+      <c r="G8" s="61">
+        <v>0</v>
+      </c>
+      <c r="H8" s="50">
+        <v>6</v>
+      </c>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="49">
+        <v>6</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="50">
+        <v>9</v>
+      </c>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="51">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="48"/>
+    </row>
+    <row r="11" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="63">
+        <v>11</v>
+      </c>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="48"/>
+    </row>
+    <row r="12" spans="1:16" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66">
+        <v>6</v>
+      </c>
+      <c r="F12" s="67">
+        <v>3</v>
+      </c>
+      <c r="G12" s="42">
+        <v>0</v>
+      </c>
+      <c r="H12" s="68">
+        <v>3</v>
+      </c>
+      <c r="I12" s="66">
+        <v>6</v>
+      </c>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="N12" s="71" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="70">
+        <f>SUM(B2:B12)</f>
+        <v>18</v>
+      </c>
+      <c r="C13" s="70">
+        <f t="shared" ref="C13:L13" si="0">SUM(C2:C12)</f>
+        <v>11</v>
+      </c>
+      <c r="D13" s="70">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="70">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F13" s="70">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G13" s="70">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H13" s="70">
+        <f>SUM(H2:H12)</f>
+        <v>18</v>
+      </c>
+      <c r="I13" s="70">
+        <f>SUM(I2:I12)</f>
+        <v>21</v>
+      </c>
+      <c r="J13" s="70">
+        <f>SUM(J2:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="70">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="L13" s="70">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="M13" s="70">
+        <f>SUM(B13:L13)</f>
+        <v>176</v>
+      </c>
+      <c r="N13" s="73">
+        <f>M13</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M14" s="72">
+        <f>M13*M13</f>
+        <v>30976</v>
+      </c>
+      <c r="N14" s="73">
+        <f>N13+M14</f>
+        <v>31152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E15" s="37"/>
+      <c r="M15" s="74">
+        <f t="shared" ref="M15:M19" si="1">M14*M14</f>
+        <v>959512576</v>
+      </c>
+      <c r="N15" s="75">
+        <f t="shared" ref="N15:N19" si="2">N14+M15</f>
+        <v>959543728</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M16" s="74">
+        <f t="shared" si="1"/>
+        <v>9.2066438350215578E+17</v>
+      </c>
+      <c r="N16" s="75">
+        <f t="shared" si="2"/>
+        <v>9.2066438446169946E+17</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M17" s="74">
+        <f t="shared" si="1"/>
+        <v>8.4762290704940455E+35</v>
+      </c>
+      <c r="N17" s="75">
+        <f t="shared" si="2"/>
+        <v>8.4762290704940455E+35</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M18" s="74">
+        <f t="shared" si="1"/>
+        <v>7.1846459255488348E+71</v>
+      </c>
+      <c r="N18" s="75">
+        <f t="shared" si="2"/>
+        <v>7.1846459255488348E+71</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M19" s="74">
+        <f t="shared" si="1"/>
+        <v>5.1619137075505474E+143</v>
+      </c>
+      <c r="N19" s="75">
+        <f t="shared" si="2"/>
+        <v>5.1619137075505474E+143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
test de capture du roi mis a jour et validé
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId1"/>
-    <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
+    <sheet name="king capture" sheetId="4" r:id="rId1"/>
+    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>3:0</t>
   </si>
@@ -148,6 +149,12 @@
   </si>
   <si>
     <t>attacker</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -170,7 +177,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,6 +208,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="23">
     <border>
@@ -520,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -632,6 +645,72 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -914,6 +993,297 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="45"/>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="48"/>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="60">
+        <v>8</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="41"/>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="55"/>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="45"/>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1239,12 +1609,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add test about the throne avoidance
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="king capture" sheetId="4" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
+    <sheet name="king capture (2)" sheetId="5" r:id="rId1"/>
+    <sheet name="king capture" sheetId="4" r:id="rId2"/>
+    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>3:0</t>
   </si>
@@ -996,7 +997,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,9 +1065,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="43"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -1099,12 +1098,8 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -1119,15 +1114,9 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="G6" s="47"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="48"/>
@@ -1139,18 +1128,10 @@
       <c r="B7" s="41"/>
       <c r="C7" s="49"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="60">
-        <v>8</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>42</v>
-      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="12" t="s">
         <v>41</v>
       </c>
@@ -1165,21 +1146,11 @@
       <c r="B8" s="53"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="55"/>
@@ -1192,15 +1163,9 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -1283,6 +1248,297 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="45"/>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="48"/>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="60">
+        <v>8</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="41"/>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="55"/>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="45"/>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -1609,7 +1865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>

</xml_diff>

<commit_message>
added test on CanMove : list count -- list detailed -- check order of pawn -- name of list under test
</commit_message>
<xml_diff>
--- a/tafl_matrice11.xlsx
+++ b/tafl_matrice11.xlsx
@@ -12,9 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="king capture" sheetId="4" r:id="rId1"/>
-    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="Feuil1" sheetId="1" r:id="rId3"/>
+    <sheet name="alone" sheetId="5" r:id="rId1"/>
+    <sheet name="king capture" sheetId="4" r:id="rId2"/>
+    <sheet name="Feuil1 (2)" sheetId="3" r:id="rId3"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>3:0</t>
   </si>
@@ -155,6 +156,9 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>1:5</t>
   </si>
 </sst>
 </file>
@@ -996,7 +1000,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,9 +1068,7 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="F3" s="12"/>
       <c r="G3" s="43"/>
       <c r="H3" s="12"/>
       <c r="I3" s="12"/>
@@ -1099,14 +1101,12 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="45"/>
     </row>
@@ -1119,15 +1119,9 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="G6" s="47"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="48"/>
@@ -1139,21 +1133,11 @@
       <c r="B7" s="41"/>
       <c r="C7" s="49"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="60">
-        <v>8</v>
-      </c>
-      <c r="H7" s="51" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="52"/>
       <c r="L7" s="41"/>
@@ -1165,21 +1149,11 @@
       <c r="B8" s="53"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="55"/>
@@ -1192,15 +1166,9 @@
       <c r="C9" s="12"/>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>41</v>
-      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -1283,6 +1251,297 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="12" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2">
+        <v>6</v>
+      </c>
+      <c r="I1" s="2">
+        <v>7</v>
+      </c>
+      <c r="J1" s="2">
+        <v>8</v>
+      </c>
+      <c r="K1" s="2">
+        <v>9</v>
+      </c>
+      <c r="L1" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="10"/>
+    </row>
+    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="14"/>
+    </row>
+    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="14"/>
+    </row>
+    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="44"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="45"/>
+    </row>
+    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="46"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="48"/>
+    </row>
+    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="41"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="60">
+        <v>8</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="41"/>
+    </row>
+    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="55"/>
+    </row>
+    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="44"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="45"/>
+    </row>
+    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="14"/>
+    </row>
+    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="14"/>
+    </row>
+    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="35"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -1609,12 +1868,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,7 +2033,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="16" t="s">

</xml_diff>